<commit_message>
First attempt at MLPRegressor
</commit_message>
<xml_diff>
--- a/FAsT-Match/Data Collection Stats.xlsx
+++ b/FAsT-Match/Data Collection Stats.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asafu\Documents\Final-Project\FAsT-Match\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4A215E5-330C-41DC-AD97-21F7268D0C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C38712F6-9B07-4015-BEF7-6C33E7143D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D54C8C64-ECA6-4324-9C20-39B4F1F66123}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D54C8C64-ECA6-4324-9C20-39B4F1F66123}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Seconds</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Computer</t>
+  </si>
+  <si>
+    <t>Number of Samples</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B639C78-9D1C-4EE0-B342-A6B732A893B3}">
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,12 +428,13 @@
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.88671875" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.77734375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -452,8 +456,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -477,8 +484,11 @@
       <c r="I2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>3616</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -502,8 +512,11 @@
       <c r="I3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K3">
+        <v>3693</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -527,8 +540,11 @@
       <c r="I4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K4">
+        <v>3969</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -552,8 +568,11 @@
       <c r="I5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K5">
+        <v>3150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -577,8 +596,11 @@
       <c r="I6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K6">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -602,8 +624,11 @@
       <c r="I7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K7">
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -627,8 +652,11 @@
       <c r="I8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K8">
+        <v>3361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -652,8 +680,11 @@
       <c r="I9">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K9">
+        <v>3550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -677,8 +708,11 @@
       <c r="I10">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K10">
+        <v>3388</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -702,8 +736,11 @@
       <c r="I11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K11">
+        <v>3197</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -727,8 +764,11 @@
       <c r="I12">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K12">
+        <v>3572</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -752,8 +792,11 @@
       <c r="I13">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K13">
+        <v>3327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -777,8 +820,11 @@
       <c r="I14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K14">
+        <v>3331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -802,8 +848,11 @@
       <c r="I15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K15">
+        <v>3624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -827,8 +876,11 @@
       <c r="I16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K16">
+        <v>3370</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -852,8 +904,11 @@
       <c r="I17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K17">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -877,8 +932,11 @@
       <c r="I18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K18">
+        <v>3484</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -902,8 +960,11 @@
       <c r="I19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K19">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -927,8 +988,11 @@
       <c r="I20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>3407</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -952,8 +1016,11 @@
       <c r="I21">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K21">
+        <v>3190</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>4</v>
       </c>
@@ -977,8 +1044,12 @@
         <f>AVERAGE(G2:G21)</f>
         <v>1354.1</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="K23">
+        <f>AVERAGE(K2:K21)</f>
+        <v>3442.7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -1001,6 +1072,10 @@
       <c r="G24">
         <f>SUM(G2:G21)</f>
         <v>27082</v>
+      </c>
+      <c r="K24">
+        <f>SUM(K2:K21)</f>
+        <v>68854</v>
       </c>
     </row>
   </sheetData>

</xml_diff>